<commit_message>
Updated to universal realm. Changed base template.
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-backport-payload-content.xlsx
+++ b/docs/StructureDefinition-backport-payload-content.xlsx
@@ -206,7 +206,7 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/subscriptions-backport/StructureDefinition/backport-payload-content</t>
+    <t>http://hl7.org/fhir/uv/subscriptions-backport/StructureDefinition/backport-payload-content</t>
   </si>
   <si>
     <t>N/A</t>
@@ -242,7 +242,7 @@
     <t>required</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/subscriptions-backport/ValueSet/backport-content-value-set</t>
+    <t>http://hl7.org/fhir/uv/subscriptions-backport/ValueSet/backport-content-value-set</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="18.9140625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="75.5546875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="75.6875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>

</xml_diff>